<commit_message>
Added visualtion to analysis python.
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -9395,20 +9395,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="19" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="22" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="17" customWidth="1" min="13" max="13"/>
-    <col width="19" customWidth="1" min="14" max="14"/>
-    <col width="17" customWidth="1" min="15" max="15"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="9" max="9"/>
+    <col width="7" customWidth="1" min="10" max="10"/>
+    <col width="9" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="14" max="14"/>
+    <col width="7" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9419,72 +9419,72 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Std Dev</t>
+          <t>SLStdDev</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Std Dev</t>
+          <t>SFStdDev</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>P-Value</t>
+          <t>PValue</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Std Dev Factor</t>
+          <t>StdDevFactor</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Count</t>
+          <t>SLCount</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Count</t>
+          <t>SLMean</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Mean</t>
+          <t>SLMedian</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Mean</t>
+          <t>SLMin</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Median</t>
+          <t>SLMax</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Median</t>
+          <t>SFCount</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Min</t>
+          <t>SFMean</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Min</t>
+          <t>SFMedian</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Locked Max</t>
+          <t>SFMin</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Syntax-Free Max</t>
+          <t>SFMax</t>
         </is>
       </c>
     </row>
@@ -9512,28 +9512,28 @@
         <v>77</v>
       </c>
       <c r="G2" t="n">
+        <v>5.012987012987013</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" t="n">
         <v>120</v>
       </c>
-      <c r="H2" t="n">
-        <v>5.012987012987013</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>4.166666666666667</v>
       </c>
-      <c r="J2" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" t="n">
-        <v>4</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
         <v>8</v>
@@ -9563,28 +9563,28 @@
         <v>77</v>
       </c>
       <c r="G3" t="n">
+        <v>3.168831168831169</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" t="n">
         <v>120</v>
       </c>
-      <c r="H3" t="n">
-        <v>3.168831168831169</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.8083333333333333</v>
       </c>
-      <c r="J3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>4</v>
@@ -9614,28 +9614,28 @@
         <v>77</v>
       </c>
       <c r="G4" t="n">
+        <v>0.935064935064935</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K4" t="n">
         <v>120</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.935064935064935</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
         <v>4</v>
@@ -9665,28 +9665,28 @@
         <v>77</v>
       </c>
       <c r="G5" t="n">
+        <v>1.194805194805195</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="n">
         <v>120</v>
       </c>
-      <c r="H5" t="n">
-        <v>1.194805194805195</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="L5" t="n">
         <v>0.7666666666666667</v>
       </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Cleaned up paper, making it more faithful to the objectives and goals actually aiming for.
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -536,7 +536,7 @@
         <v>10519</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
@@ -9495,24 +9495,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.810012405406067</v>
+        <v>1.806232091326451</v>
       </c>
       <c r="C2" t="n">
         <v>0.8130586853175534</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.000205</t>
+          <t>0.000162</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2.226176828427995</v>
+        <v>2.221527331229477</v>
       </c>
       <c r="F2" t="n">
         <v>77</v>
       </c>
       <c r="G2" t="n">
-        <v>5.012987012987013</v>
+        <v>5.025974025974026</v>
       </c>
       <c r="H2" t="n">
         <v>5</v>

</xml_diff>